<commit_message>
dataset + code cmc
</commit_message>
<xml_diff>
--- a/Documentazione/DATI SITI/Companies market cap/dati.xlsx
+++ b/Documentazione/DATI SITI/Companies market cap/dati.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Wissel\OneDrive\Desktop\università\MAGISTRALE\Ing.Dati\Homework 5- repo\Web-Scraping-homework5\Documentazione\DATI SITI\Companies market cap\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Web-Scraping-homework5\Documentazione\DATI SITI\Companies market cap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC802536-74DB-4ECE-8B81-507EBFC637EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D95CE416-8BF5-44E4-B630-C346D907F238}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0045C306-CACA-4588-A826-E9BE569D0A38}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{0045C306-CACA-4588-A826-E9BE569D0A38}"/>
   </bookViews>
   <sheets>
     <sheet name="market cap" sheetId="1" r:id="rId1"/>
@@ -26,9 +26,6 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -269,9 +266,6 @@
   </cellStyleXfs>
   <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -280,6 +274,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -612,185 +609,185 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="67.5546875" customWidth="1"/>
-    <col min="3" max="3" width="20.33203125" customWidth="1"/>
-    <col min="4" max="4" width="23.33203125" customWidth="1"/>
+    <col min="1" max="1" width="25.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="67.54296875" customWidth="1"/>
+    <col min="3" max="3" width="20.36328125" customWidth="1"/>
+    <col min="4" max="4" width="23.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="C2" s="1"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="2"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
+      <c r="C3" s="1"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-    </row>
-    <row r="6" spans="1:4" ht="21" x14ac:dyDescent="0.4">
-      <c r="A6" s="3" t="s">
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+    </row>
+    <row r="6" spans="1:4" ht="21" x14ac:dyDescent="0.5">
+      <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
       <c r="D7" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="2"/>
+      <c r="C8" s="1"/>
       <c r="D8" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="2"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
+      <c r="C9" s="1"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="2"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
+      <c r="C10" s="1"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="2"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
+      <c r="C11" s="1"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="2"/>
+      <c r="C12" s="1"/>
       <c r="D12" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C13" s="2"/>
+      <c r="C13" s="1"/>
       <c r="D13" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="6" t="s">
         <v>31</v>
       </c>
       <c r="B14" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C14" s="2"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C14" s="1"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="7"/>
       <c r="B15" s="9"/>
-      <c r="C15" s="2"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C15" s="1"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="7"/>
       <c r="B16" s="9"/>
-      <c r="C16" s="2"/>
+      <c r="C16" s="1"/>
       <c r="D16" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="7"/>
       <c r="B17" s="10"/>
-      <c r="C17" s="2"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="5" t="s">
+      <c r="C17" s="1"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="5" t="s">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="5" t="s">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A22" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="5" t="s">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A23" s="4" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>